<commit_message>
fix: quản lý đơn nghỉ phép, xuất báo cáo
</commit_message>
<xml_diff>
--- a/src/main/resources/excel-template/export-leave-template.xlsx
+++ b/src/main/resources/excel-template/export-leave-template.xlsx
@@ -80,10 +80,10 @@
     <t>${item.leaveCategory}</t>
   </si>
   <si>
-    <t>${item.startDay}</t>
-  </si>
-  <si>
-    <t>${item.endDay}</t>
+    <t>${item.startDayConvert}</t>
+  </si>
+  <si>
+    <t>${item.endDayConvert}</t>
   </si>
   <si>
     <t>${item.description}</t>
@@ -95,7 +95,7 @@
     <t>${item.trackerName}</t>
   </si>
   <si>
-    <t>${item.isActive}</t>
+    <t>${item.isActiveName}</t>
   </si>
   <si>
     <t>&lt;/jx:forEach&gt;</t>
@@ -1117,8 +1117,8 @@
   <sheetPr/>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="14.4" outlineLevelRow="6"/>
@@ -1127,7 +1127,7 @@
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="27.4444444444444" customWidth="1"/>
     <col min="4" max="4" width="21.7777777777778" customWidth="1"/>
-    <col min="5" max="5" width="19.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="22.5555555555556" customWidth="1"/>
     <col min="6" max="6" width="39" customWidth="1"/>
     <col min="7" max="7" width="20.7777777777778" customWidth="1"/>
     <col min="8" max="8" width="23.4444444444444" customWidth="1"/>

</xml_diff>